<commit_message>
updated onenCart RTM file added
</commit_message>
<xml_diff>
--- a/OpenCart-RTM.xlsx
+++ b/OpenCart-RTM.xlsx
@@ -1,87 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Full Stack QA_05-Jan-2021\Day11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A505EC97-D8B0-4AB0-AB84-F75DC257E5C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F514701B-12A4-488D-9F05-E4003739F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1800" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Project Name</t>
   </si>
   <si>
+    <t>OpenCart (Frontend)</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>OpenCart</t>
+  </si>
+  <si>
     <t>Reference Document</t>
   </si>
   <si>
+    <t>FRS</t>
+  </si>
+  <si>
     <t>Created By</t>
   </si>
   <si>
+    <t>GM Rajon</t>
+  </si>
+  <si>
     <t>Creation Date</t>
   </si>
   <si>
+    <t>Approval Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Requirement ID</t>
+  </si>
+  <si>
     <t>Test Scenario ID</t>
   </si>
   <si>
     <t>Test Scenario Description</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Approval Date</t>
+    <t>Tes Case ID'S</t>
   </si>
   <si>
     <t>TS_001</t>
   </si>
   <si>
-    <t>TS_002</t>
-  </si>
-  <si>
-    <t>OpenCart (Frontend)</t>
-  </si>
-  <si>
-    <t>OpenCart</t>
-  </si>
-  <si>
-    <t>Pavan</t>
-  </si>
-  <si>
     <t>Validate the working of Register Account functionality</t>
-  </si>
-  <si>
-    <t>Validate the working of Login functionality</t>
-  </si>
-  <si>
-    <t>FRS</t>
-  </si>
-  <si>
-    <t>DD-MM-YYYY</t>
-  </si>
-  <si>
-    <t>Tes Case ID'S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Requirement ID</t>
   </si>
   <si>
     <t xml:space="preserve">TC_RF_001
@@ -114,6 +116,12 @@
 </t>
   </si>
   <si>
+    <t>TS_002</t>
+  </si>
+  <si>
+    <t>Validate the working of Login functionality</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_LF_001
 TC_LF_002
 TC_LF_003
@@ -139,12 +147,126 @@
 TC_LF_023
 </t>
   </si>
+  <si>
+    <t>TS_003</t>
+  </si>
+  <si>
+    <t>Validate the working of Logout functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_LF_001
+TC_LF_002
+TC_LF_003
+TC_LF_004
+TC_LF_005
+TC_LF_006
+TC_LF_007
+TC_LF_008
+TC_LF_009
+TC_LF_010
+TC_LF_011
+</t>
+  </si>
+  <si>
+    <t>TS_004</t>
+  </si>
+  <si>
+    <t>Validate the working of Forgot Password functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_FPF_001
+TC_FPF_002
+TC_FPF_003
+TC_FPF_004
+TC_FPF_005
+TC_FPF_006
+TC_FPF_007
+TC_FPF_008
+TC_FPF_009
+TC_FPF_010
+TC_FPF_011
+TC_FPF_012
+TC_FPF_013
+TC_FPF_014
+TC_FPF_015
+TC_FPF_016
+TC_FPF_017
+TC_FPF_018
+TC_FPF_019
+TC_FPF_020
+TC_FPF_021
+TC_FPF_022
+TC_FPF_023
+TC_FPF_024
+TC_FPF_025
+</t>
+  </si>
+  <si>
+    <t>TS_005</t>
+  </si>
+  <si>
+    <t>Validate the working of Seacrch functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_SF_001
+TC_SF_002
+TC_SF_003
+TC_SF_004
+TC_SF_005
+TC_SF_006
+TC_SF_007
+TC_SF_008
+TC_SF_009
+TC_SF_010
+TC_SF_011
+TC_SF_012
+TC_SF_013
+TC_SF_014
+TC_SF_015
+TC_SF_016
+TC_SF_017
+TC_SF_018
+TC_SF_019
+TC_SF_020
+TC_SF_021
+</t>
+  </si>
+  <si>
+    <t>TS_006</t>
+  </si>
+  <si>
+    <t>Validate the working of Product compare functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_PCF_001
+TC_PCF_002
+TC_PCF_003
+TC_PCF_004
+TC_PCF_005
+TC_PCF_006
+TC_PCF_007
+TC_PCF_008
+TC_PCF_009
+TC_PCF_010
+TC_PCF_011
+TC_PCF_012
+TC_PCF_013
+TC_PCF_014
+TC_PCF_015
+TC_PCF_016
+TC_PCF_017
+TC_PCF_018
+TC_PCF_019
+TC_PCF_020
+TC_PCF_021
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -328,16 +450,34 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -620,13 +760,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
@@ -635,103 +775,159 @@
     <col min="5" max="16384" width="31.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12">
+        <v>45874</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="12">
+        <v>45905</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="352.5">
+      <c r="A11" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="D11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="302.25">
+      <c r="A12" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="357" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="306" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1.2</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="13" t="s">
+    <row r="13" spans="1:4" ht="163.5">
+      <c r="A13" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="340.5">
+      <c r="A14" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="277.5">
+      <c r="A15" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="277.5">
+      <c r="A16" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>